<commit_message>
Update PDF and Excel templates
</commit_message>
<xml_diff>
--- a/clients/ArrowHead/data/template/Workbooktemplate.xlsx
+++ b/clients/ArrowHead/data/template/Workbooktemplate.xlsx
@@ -340,10 +340,10 @@
     <t xml:space="preserve">Utilities Options:</t>
   </si>
   <si>
+    <t xml:space="preserve">Water Supply</t>
+  </si>
+  <si>
     <t xml:space="preserve">{utilityoptions}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Supply</t>
   </si>
   <si>
     <t xml:space="preserve">Communication Supply</t>
@@ -1487,7 +1487,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1521,6 +1521,17 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -1587,7 +1598,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1609,6 +1620,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1699,11 +1718,11 @@
   </sheetPr>
   <dimension ref="A1:J292"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B80" activeCellId="0" sqref="B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.83"/>
@@ -2153,12 +2172,13 @@
       <c r="A79" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B79" s="0" t="s">
-        <v>106</v>
-      </c>
+      <c r="B79" s="6"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" s="7" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2166,6 +2186,7 @@
       <c r="A81" s="0" t="s">
         <v>108</v>
       </c>
+      <c r="B81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
@@ -2763,16 +2784,16 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B163" s="6" t="s">
+      <c r="B163" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C163" s="6"/>
-      <c r="D163" s="6"/>
-      <c r="E163" s="7" t="s">
+      <c r="C163" s="8"/>
+      <c r="D163" s="8"/>
+      <c r="E163" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F163" s="7"/>
-      <c r="G163" s="7"/>
+      <c r="F163" s="9"/>
+      <c r="G163" s="9"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">

</xml_diff>